<commit_message>
Auto-load Excel files for dashboard
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amit2\OneDrive\Desktop\DESKTOP\NEW DATA\usb data\DAILYWORKING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amit2\OneDrive\Desktop\DESKTOP\NEW DATA\usb data\orders_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B05B4DA-E76F-44C4-B1EB-D922F4C5AC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4BB84E-5B7C-4994-99BA-87E866751FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10774" uniqueCount="2274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10658" uniqueCount="2275">
   <si>
     <t>Date</t>
   </si>
@@ -6877,6 +6877,9 @@
   </si>
   <si>
     <t>8899000063</t>
+  </si>
+  <si>
+    <t>Order Date</t>
   </si>
 </sst>
 </file>
@@ -7424,7 +7427,7 @@
   <sheetData>
     <row r="1" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>0</v>
+        <v>2274</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1369</v>
@@ -7704,8 +7707,8 @@
       </c>
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>1454</v>
+      <c r="A2" s="4">
+        <v>45901</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>1455</v>
@@ -7949,8 +7952,8 @@
       <c r="CO2" s="19"/>
     </row>
     <row r="3" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>1454</v>
+      <c r="A3" s="4">
+        <v>45901</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>1455</v>
@@ -8194,8 +8197,8 @@
       <c r="CO3" s="19"/>
     </row>
     <row r="4" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>1454</v>
+      <c r="A4" s="4">
+        <v>45901</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>1455</v>
@@ -8441,8 +8444,8 @@
       <c r="CO4" s="19"/>
     </row>
     <row r="5" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>1454</v>
+      <c r="A5" s="4">
+        <v>45901</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>1498</v>
@@ -8678,8 +8681,8 @@
       <c r="CO5" s="19"/>
     </row>
     <row r="6" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>1454</v>
+      <c r="A6" s="4">
+        <v>45901</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>1455</v>
@@ -8917,8 +8920,8 @@
       <c r="CO6" s="19"/>
     </row>
     <row r="7" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>1454</v>
+      <c r="A7" s="4">
+        <v>45901</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>1498</v>
@@ -9154,8 +9157,8 @@
       <c r="CO7" s="19"/>
     </row>
     <row r="8" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>1454</v>
+      <c r="A8" s="4">
+        <v>45901</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>1498</v>
@@ -9391,8 +9394,8 @@
       <c r="CO8" s="19"/>
     </row>
     <row r="9" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>1454</v>
+      <c r="A9" s="4">
+        <v>45901</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>1455</v>
@@ -9616,8 +9619,8 @@
       <c r="CO9" s="19"/>
     </row>
     <row r="10" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>1454</v>
+      <c r="A10" s="4">
+        <v>45901</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>1532</v>
@@ -9875,8 +9878,8 @@
       </c>
     </row>
     <row r="11" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>1454</v>
+      <c r="A11" s="4">
+        <v>45901</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>1455</v>
@@ -10102,8 +10105,8 @@
       <c r="CO11" s="19"/>
     </row>
     <row r="12" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>1454</v>
+      <c r="A12" s="4">
+        <v>45901</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>502</v>
@@ -10335,8 +10338,8 @@
       <c r="CO12" s="19"/>
     </row>
     <row r="13" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>1454</v>
+      <c r="A13" s="4">
+        <v>45901</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>1498</v>
@@ -10584,8 +10587,8 @@
       <c r="CO13" s="19"/>
     </row>
     <row r="14" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>1454</v>
+      <c r="A14" s="4">
+        <v>45901</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>502</v>
@@ -10835,8 +10838,8 @@
       <c r="CO14" s="19"/>
     </row>
     <row r="15" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>1454</v>
+      <c r="A15" s="4">
+        <v>45901</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>1532</v>
@@ -11074,8 +11077,8 @@
       <c r="CO15" s="19"/>
     </row>
     <row r="16" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>1454</v>
+      <c r="A16" s="4">
+        <v>45901</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>502</v>
@@ -11323,8 +11326,8 @@
       <c r="CO16" s="19"/>
     </row>
     <row r="17" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>1454</v>
+      <c r="A17" s="4">
+        <v>45901</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>502</v>
@@ -11572,8 +11575,8 @@
       <c r="CO17" s="19"/>
     </row>
     <row r="18" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>1454</v>
+      <c r="A18" s="4">
+        <v>45901</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>1498</v>
@@ -11833,8 +11836,8 @@
       </c>
     </row>
     <row r="19" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>1454</v>
+      <c r="A19" s="4">
+        <v>45901</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>1498</v>
@@ -12064,8 +12067,8 @@
       <c r="CO19" s="19"/>
     </row>
     <row r="20" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>1454</v>
+      <c r="A20" s="4">
+        <v>45901</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>1532</v>
@@ -12301,8 +12304,8 @@
       <c r="CO20" s="19"/>
     </row>
     <row r="21" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>1454</v>
+      <c r="A21" s="4">
+        <v>45901</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>1498</v>
@@ -12532,8 +12535,8 @@
       <c r="CO21" s="19"/>
     </row>
     <row r="22" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>1454</v>
+      <c r="A22" s="4">
+        <v>45901</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>502</v>
@@ -12763,8 +12766,8 @@
       <c r="CO22" s="19"/>
     </row>
     <row r="23" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>1454</v>
+      <c r="A23" s="4">
+        <v>45901</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>502</v>
@@ -12994,8 +12997,8 @@
       <c r="CO23" s="19"/>
     </row>
     <row r="24" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>1454</v>
+      <c r="A24" s="4">
+        <v>45901</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>502</v>
@@ -13225,8 +13228,8 @@
       <c r="CO24" s="19"/>
     </row>
     <row r="25" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>1454</v>
+      <c r="A25" s="4">
+        <v>45901</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>502</v>
@@ -13456,8 +13459,8 @@
       <c r="CO25" s="19"/>
     </row>
     <row r="26" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>1454</v>
+      <c r="A26" s="4">
+        <v>45901</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>502</v>
@@ -13687,8 +13690,8 @@
       <c r="CO26" s="19"/>
     </row>
     <row r="27" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>1454</v>
+      <c r="A27" s="4">
+        <v>45901</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>1498</v>
@@ -13940,8 +13943,8 @@
       <c r="CO27" s="19"/>
     </row>
     <row r="28" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>1454</v>
+      <c r="A28" s="4">
+        <v>45901</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>1498</v>
@@ -14183,8 +14186,8 @@
       <c r="CO28" s="19"/>
     </row>
     <row r="29" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>1454</v>
+      <c r="A29" s="4">
+        <v>45901</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>1498</v>
@@ -14416,8 +14419,8 @@
       <c r="CO29" s="19"/>
     </row>
     <row r="30" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>1454</v>
+      <c r="A30" s="4">
+        <v>45901</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>1498</v>
@@ -14651,8 +14654,8 @@
       <c r="CO30" s="19"/>
     </row>
     <row r="31" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>1454</v>
+      <c r="A31" s="4">
+        <v>45901</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>1498</v>
@@ -14888,8 +14891,8 @@
       <c r="CO31" s="19"/>
     </row>
     <row r="32" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>1454</v>
+      <c r="A32" s="4">
+        <v>45901</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>502</v>
@@ -15121,8 +15124,8 @@
       <c r="CO32" s="19"/>
     </row>
     <row r="33" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>1454</v>
+      <c r="A33" s="4">
+        <v>45901</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>1498</v>
@@ -15374,8 +15377,8 @@
       </c>
     </row>
     <row r="34" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>1454</v>
+      <c r="A34" s="4">
+        <v>45901</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>1498</v>
@@ -15605,8 +15608,8 @@
       <c r="CO34" s="19"/>
     </row>
     <row r="35" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>1454</v>
+      <c r="A35" s="4">
+        <v>45901</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>1455</v>
@@ -15840,8 +15843,8 @@
       <c r="CO35" s="19"/>
     </row>
     <row r="36" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>1454</v>
+      <c r="A36" s="4">
+        <v>45901</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>1455</v>
@@ -16087,8 +16090,8 @@
       <c r="CO36" s="19"/>
     </row>
     <row r="37" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>1454</v>
+      <c r="A37" s="4">
+        <v>45901</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>1532</v>
@@ -16322,8 +16325,8 @@
       <c r="CO37" s="19"/>
     </row>
     <row r="38" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>1454</v>
+      <c r="A38" s="4">
+        <v>45901</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>1532</v>
@@ -16555,8 +16558,8 @@
       <c r="CO38" s="19"/>
     </row>
     <row r="39" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>1454</v>
+      <c r="A39" s="4">
+        <v>45901</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>1532</v>
@@ -16792,8 +16795,8 @@
       <c r="CO39" s="19"/>
     </row>
     <row r="40" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>1454</v>
+      <c r="A40" s="4">
+        <v>45901</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>1532</v>
@@ -17035,8 +17038,8 @@
       <c r="CO40" s="19"/>
     </row>
     <row r="41" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>1454</v>
+      <c r="A41" s="4">
+        <v>45901</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>1532</v>
@@ -17268,8 +17271,8 @@
       <c r="CO41" s="19"/>
     </row>
     <row r="42" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>1454</v>
+      <c r="A42" s="4">
+        <v>45901</v>
       </c>
       <c r="B42" s="19" t="s">
         <v>1532</v>
@@ -17509,8 +17512,8 @@
       <c r="CO42" s="19"/>
     </row>
     <row r="43" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>1454</v>
+      <c r="A43" s="4">
+        <v>45901</v>
       </c>
       <c r="B43" s="19" t="s">
         <v>1532</v>
@@ -17774,8 +17777,8 @@
       </c>
     </row>
     <row r="44" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>1454</v>
+      <c r="A44" s="4">
+        <v>45901</v>
       </c>
       <c r="B44" s="19" t="s">
         <v>502</v>
@@ -18007,8 +18010,8 @@
       <c r="CO44" s="19"/>
     </row>
     <row r="45" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>1454</v>
+      <c r="A45" s="4">
+        <v>45901</v>
       </c>
       <c r="B45" s="19" t="s">
         <v>1498</v>
@@ -18260,8 +18263,8 @@
       <c r="CO45" s="19"/>
     </row>
     <row r="46" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>1454</v>
+      <c r="A46" s="4">
+        <v>45901</v>
       </c>
       <c r="B46" s="19" t="s">
         <v>1532</v>
@@ -18517,8 +18520,8 @@
       </c>
     </row>
     <row r="47" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>1454</v>
+      <c r="A47" s="4">
+        <v>45901</v>
       </c>
       <c r="B47" s="19" t="s">
         <v>1532</v>
@@ -18774,8 +18777,8 @@
       <c r="CO47" s="19"/>
     </row>
     <row r="48" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>1454</v>
+      <c r="A48" s="4">
+        <v>45901</v>
       </c>
       <c r="B48" s="19" t="s">
         <v>1532</v>
@@ -19027,8 +19030,8 @@
       <c r="CO48" s="19"/>
     </row>
     <row r="49" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>1454</v>
+      <c r="A49" s="4">
+        <v>45901</v>
       </c>
       <c r="B49" s="19" t="s">
         <v>1532</v>
@@ -19262,8 +19265,8 @@
       <c r="CO49" s="19"/>
     </row>
     <row r="50" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>1454</v>
+      <c r="A50" s="4">
+        <v>45901</v>
       </c>
       <c r="B50" s="19" t="s">
         <v>1498</v>
@@ -19513,8 +19516,8 @@
       <c r="CO50" s="19"/>
     </row>
     <row r="51" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>1454</v>
+      <c r="A51" s="4">
+        <v>45901</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>1498</v>
@@ -19748,8 +19751,8 @@
       <c r="CO51" s="19"/>
     </row>
     <row r="52" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>1454</v>
+      <c r="A52" s="4">
+        <v>45901</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>1532</v>
@@ -19985,8 +19988,8 @@
       <c r="CO52" s="19"/>
     </row>
     <row r="53" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>1454</v>
+      <c r="A53" s="4">
+        <v>45901</v>
       </c>
       <c r="B53" s="19" t="s">
         <v>1532</v>
@@ -20242,8 +20245,8 @@
       </c>
     </row>
     <row r="54" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>1454</v>
+      <c r="A54" s="4">
+        <v>45901</v>
       </c>
       <c r="B54" s="19" t="s">
         <v>1498</v>
@@ -20477,8 +20480,8 @@
       <c r="CO54" s="19"/>
     </row>
     <row r="55" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>1454</v>
+      <c r="A55" s="4">
+        <v>45901</v>
       </c>
       <c r="B55" s="19" t="s">
         <v>1532</v>
@@ -20714,8 +20717,8 @@
       <c r="CO55" s="19"/>
     </row>
     <row r="56" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
-        <v>1454</v>
+      <c r="A56" s="4">
+        <v>45901</v>
       </c>
       <c r="B56" s="19" t="s">
         <v>1532</v>
@@ -20969,8 +20972,8 @@
       <c r="CO56" s="19"/>
     </row>
     <row r="57" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>1454</v>
+      <c r="A57" s="4">
+        <v>45901</v>
       </c>
       <c r="B57" s="19" t="s">
         <v>1532</v>
@@ -21206,8 +21209,8 @@
       <c r="CO57" s="19"/>
     </row>
     <row r="58" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>1454</v>
+      <c r="A58" s="4">
+        <v>45901</v>
       </c>
       <c r="B58" s="19" t="s">
         <v>502</v>
@@ -21439,8 +21442,8 @@
       <c r="CO58" s="19"/>
     </row>
     <row r="59" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>1454</v>
+      <c r="A59" s="4">
+        <v>45901</v>
       </c>
       <c r="B59" s="19" t="s">
         <v>1498</v>
@@ -21674,8 +21677,8 @@
       <c r="CO59" s="19"/>
     </row>
     <row r="60" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>1454</v>
+      <c r="A60" s="4">
+        <v>45901</v>
       </c>
       <c r="B60" s="19" t="s">
         <v>1532</v>
@@ -21913,8 +21916,8 @@
       <c r="CO60" s="19"/>
     </row>
     <row r="61" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>1454</v>
+      <c r="A61" s="4">
+        <v>45901</v>
       </c>
       <c r="B61" s="19" t="s">
         <v>1498</v>
@@ -22150,8 +22153,8 @@
       <c r="CO61" s="19"/>
     </row>
     <row r="62" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>1454</v>
+      <c r="A62" s="4">
+        <v>45901</v>
       </c>
       <c r="B62" s="19" t="s">
         <v>502</v>
@@ -22403,8 +22406,8 @@
       <c r="CO62" s="19"/>
     </row>
     <row r="63" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
-        <v>1454</v>
+      <c r="A63" s="4">
+        <v>45901</v>
       </c>
       <c r="B63" s="19" t="s">
         <v>502</v>
@@ -22640,8 +22643,8 @@
       <c r="CO63" s="19"/>
     </row>
     <row r="64" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
-        <v>1454</v>
+      <c r="A64" s="4">
+        <v>45901</v>
       </c>
       <c r="B64" s="19" t="s">
         <v>502</v>
@@ -22893,8 +22896,8 @@
       </c>
     </row>
     <row r="65" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
-        <v>1454</v>
+      <c r="A65" s="4">
+        <v>45901</v>
       </c>
       <c r="B65" s="19" t="s">
         <v>502</v>
@@ -23142,8 +23145,8 @@
       <c r="CO65" s="19"/>
     </row>
     <row r="66" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>1454</v>
+      <c r="A66" s="4">
+        <v>45901</v>
       </c>
       <c r="B66" s="19" t="s">
         <v>502</v>
@@ -23379,8 +23382,8 @@
       <c r="CO66" s="19"/>
     </row>
     <row r="67" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>1454</v>
+      <c r="A67" s="4">
+        <v>45901</v>
       </c>
       <c r="B67" s="19" t="s">
         <v>502</v>
@@ -23628,8 +23631,8 @@
       <c r="CO67" s="19"/>
     </row>
     <row r="68" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
-        <v>1454</v>
+      <c r="A68" s="4">
+        <v>45901</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>1455</v>
@@ -23857,8 +23860,8 @@
       <c r="CO68" s="19"/>
     </row>
     <row r="69" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>1454</v>
+      <c r="A69" s="4">
+        <v>45901</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>1498</v>
@@ -24092,8 +24095,8 @@
       <c r="CO69" s="19"/>
     </row>
     <row r="70" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
-        <v>1454</v>
+      <c r="A70" s="4">
+        <v>45901</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>1498</v>
@@ -24327,8 +24330,8 @@
       <c r="CO70" s="19"/>
     </row>
     <row r="71" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
-        <v>1454</v>
+      <c r="A71" s="4">
+        <v>45901</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>1498</v>
@@ -24584,8 +24587,8 @@
       <c r="CO71" s="19"/>
     </row>
     <row r="72" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A72" s="4" t="s">
-        <v>1454</v>
+      <c r="A72" s="4">
+        <v>45901</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>1498</v>
@@ -24841,8 +24844,8 @@
       <c r="CO72" s="19"/>
     </row>
     <row r="73" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
-        <v>1454</v>
+      <c r="A73" s="4">
+        <v>45901</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>502</v>
@@ -25078,8 +25081,8 @@
       <c r="CO73" s="19"/>
     </row>
     <row r="74" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A74" s="4" t="s">
-        <v>1454</v>
+      <c r="A74" s="4">
+        <v>45901</v>
       </c>
       <c r="B74" s="19" t="s">
         <v>1532</v>
@@ -25335,8 +25338,8 @@
       </c>
     </row>
     <row r="75" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>1454</v>
+      <c r="A75" s="4">
+        <v>45901</v>
       </c>
       <c r="B75" s="19" t="s">
         <v>1532</v>
@@ -25588,8 +25591,8 @@
       </c>
     </row>
     <row r="76" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A76" s="4" t="s">
-        <v>1454</v>
+      <c r="A76" s="4">
+        <v>45901</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>1532</v>
@@ -25845,8 +25848,8 @@
       </c>
     </row>
     <row r="77" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="s">
-        <v>1454</v>
+      <c r="A77" s="4">
+        <v>45901</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>1498</v>
@@ -26078,8 +26081,8 @@
       <c r="CO77" s="19"/>
     </row>
     <row r="78" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
-        <v>1454</v>
+      <c r="A78" s="4">
+        <v>45901</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>1532</v>
@@ -26317,8 +26320,8 @@
       <c r="CO78" s="19"/>
     </row>
     <row r="79" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
-        <v>1454</v>
+      <c r="A79" s="4">
+        <v>45901</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>1532</v>
@@ -26556,8 +26559,8 @@
       <c r="CO79" s="19"/>
     </row>
     <row r="80" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A80" s="4" t="s">
-        <v>1454</v>
+      <c r="A80" s="4">
+        <v>45901</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>1532</v>
@@ -26811,8 +26814,8 @@
       </c>
     </row>
     <row r="81" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="s">
-        <v>1454</v>
+      <c r="A81" s="4">
+        <v>45901</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>1532</v>
@@ -27068,8 +27071,8 @@
       <c r="CO81" s="19"/>
     </row>
     <row r="82" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>1454</v>
+      <c r="A82" s="4">
+        <v>45901</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>1532</v>
@@ -27327,8 +27330,8 @@
       <c r="CO82" s="19"/>
     </row>
     <row r="83" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="s">
-        <v>1454</v>
+      <c r="A83" s="4">
+        <v>45901</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>502</v>
@@ -27586,8 +27589,8 @@
       <c r="CO83" s="19"/>
     </row>
     <row r="84" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A84" s="4" t="s">
-        <v>1454</v>
+      <c r="A84" s="4">
+        <v>45901</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>502</v>
@@ -27825,8 +27828,8 @@
       <c r="CO84" s="19"/>
     </row>
     <row r="85" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>1454</v>
+      <c r="A85" s="4">
+        <v>45901</v>
       </c>
       <c r="B85" s="19" t="s">
         <v>1532</v>
@@ -28062,8 +28065,8 @@
       <c r="CO85" s="19"/>
     </row>
     <row r="86" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A86" s="4" t="s">
-        <v>1454</v>
+      <c r="A86" s="4">
+        <v>45901</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>1532</v>
@@ -28295,8 +28298,8 @@
       <c r="CO86" s="19"/>
     </row>
     <row r="87" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
-        <v>1454</v>
+      <c r="A87" s="4">
+        <v>45901</v>
       </c>
       <c r="B87" s="19" t="s">
         <v>502</v>
@@ -28534,8 +28537,8 @@
       <c r="CO87" s="19"/>
     </row>
     <row r="88" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
-        <v>1454</v>
+      <c r="A88" s="4">
+        <v>45901</v>
       </c>
       <c r="B88" s="19" t="s">
         <v>502</v>
@@ -28771,8 +28774,8 @@
       <c r="CO88" s="19"/>
     </row>
     <row r="89" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
-        <v>1454</v>
+      <c r="A89" s="4">
+        <v>45901</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>502</v>
@@ -29022,8 +29025,8 @@
       <c r="CO89" s="19"/>
     </row>
     <row r="90" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
-        <v>1454</v>
+      <c r="A90" s="4">
+        <v>45901</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>502</v>
@@ -29271,8 +29274,8 @@
       </c>
     </row>
     <row r="91" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A91" s="4" t="s">
-        <v>1454</v>
+      <c r="A91" s="4">
+        <v>45901</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>1498</v>
@@ -29512,8 +29515,8 @@
       <c r="CO91" s="19"/>
     </row>
     <row r="92" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A92" s="4" t="s">
-        <v>1454</v>
+      <c r="A92" s="4">
+        <v>45901</v>
       </c>
       <c r="B92" s="19" t="s">
         <v>1498</v>
@@ -29749,8 +29752,8 @@
       <c r="CO92" s="19"/>
     </row>
     <row r="93" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A93" s="4" t="s">
-        <v>1454</v>
+      <c r="A93" s="4">
+        <v>45901</v>
       </c>
       <c r="B93" s="19" t="s">
         <v>1498</v>
@@ -30002,8 +30005,8 @@
       <c r="CO93" s="19"/>
     </row>
     <row r="94" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A94" s="4" t="s">
-        <v>1454</v>
+      <c r="A94" s="4">
+        <v>45901</v>
       </c>
       <c r="B94" s="19" t="s">
         <v>1498</v>
@@ -30237,8 +30240,8 @@
       <c r="CO94" s="19"/>
     </row>
     <row r="95" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A95" s="4" t="s">
-        <v>1454</v>
+      <c r="A95" s="4">
+        <v>45901</v>
       </c>
       <c r="B95" s="19" t="s">
         <v>1498</v>
@@ -30472,8 +30475,8 @@
       <c r="CO95" s="19"/>
     </row>
     <row r="96" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A96" s="4" t="s">
-        <v>1454</v>
+      <c r="A96" s="4">
+        <v>45901</v>
       </c>
       <c r="B96" s="19" t="s">
         <v>502</v>
@@ -30707,8 +30710,8 @@
       <c r="CO96" s="19"/>
     </row>
     <row r="97" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
-        <v>1454</v>
+      <c r="A97" s="4">
+        <v>45901</v>
       </c>
       <c r="B97" s="19" t="s">
         <v>502</v>
@@ -30940,8 +30943,8 @@
       <c r="CO97" s="19"/>
     </row>
     <row r="98" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
-        <v>1454</v>
+      <c r="A98" s="4">
+        <v>45901</v>
       </c>
       <c r="B98" s="19" t="s">
         <v>1532</v>
@@ -31195,8 +31198,8 @@
       <c r="CO98" s="19"/>
     </row>
     <row r="99" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
-        <v>1454</v>
+      <c r="A99" s="4">
+        <v>45901</v>
       </c>
       <c r="B99" s="19" t="s">
         <v>1532</v>
@@ -31448,8 +31451,8 @@
       <c r="CO99" s="19"/>
     </row>
     <row r="100" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A100" s="4" t="s">
-        <v>1454</v>
+      <c r="A100" s="4">
+        <v>45901</v>
       </c>
       <c r="B100" s="19" t="s">
         <v>1498</v>
@@ -31683,8 +31686,8 @@
       <c r="CO100" s="19"/>
     </row>
     <row r="101" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="s">
-        <v>1454</v>
+      <c r="A101" s="4">
+        <v>45901</v>
       </c>
       <c r="B101" s="19" t="s">
         <v>1498</v>
@@ -31914,8 +31917,8 @@
       <c r="CO101" s="19"/>
     </row>
     <row r="102" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>1454</v>
+      <c r="A102" s="4">
+        <v>45901</v>
       </c>
       <c r="B102" s="19" t="s">
         <v>1498</v>
@@ -32151,8 +32154,8 @@
       <c r="CO102" s="19"/>
     </row>
     <row r="103" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
-        <v>1454</v>
+      <c r="A103" s="4">
+        <v>45901</v>
       </c>
       <c r="B103" s="19" t="s">
         <v>1498</v>
@@ -32402,8 +32405,8 @@
       <c r="CO103" s="19"/>
     </row>
     <row r="104" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>1454</v>
+      <c r="A104" s="4">
+        <v>45901</v>
       </c>
       <c r="B104" s="19" t="s">
         <v>1498</v>
@@ -32635,8 +32638,8 @@
       <c r="CO104" s="19"/>
     </row>
     <row r="105" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
-        <v>1454</v>
+      <c r="A105" s="4">
+        <v>45901</v>
       </c>
       <c r="B105" s="19" t="s">
         <v>1498</v>
@@ -32876,8 +32879,8 @@
       <c r="CO105" s="19"/>
     </row>
     <row r="106" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
-        <v>1454</v>
+      <c r="A106" s="4">
+        <v>45901</v>
       </c>
       <c r="B106" s="19" t="s">
         <v>1498</v>
@@ -33107,8 +33110,8 @@
       <c r="CO106" s="19"/>
     </row>
     <row r="107" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>1454</v>
+      <c r="A107" s="4">
+        <v>45901</v>
       </c>
       <c r="B107" s="19" t="s">
         <v>1498</v>
@@ -33356,8 +33359,8 @@
       </c>
     </row>
     <row r="108" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
-        <v>1454</v>
+      <c r="A108" s="4">
+        <v>45901</v>
       </c>
       <c r="B108" s="19" t="s">
         <v>1498</v>
@@ -33591,8 +33594,8 @@
       <c r="CO108" s="19"/>
     </row>
     <row r="109" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
-        <v>1454</v>
+      <c r="A109" s="4">
+        <v>45901</v>
       </c>
       <c r="B109" s="19" t="s">
         <v>1498</v>
@@ -33846,8 +33849,8 @@
       <c r="CO109" s="19"/>
     </row>
     <row r="110" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A110" s="4" t="s">
-        <v>1454</v>
+      <c r="A110" s="4">
+        <v>45901</v>
       </c>
       <c r="B110" s="19" t="s">
         <v>1498</v>
@@ -34083,8 +34086,8 @@
       <c r="CO110" s="19"/>
     </row>
     <row r="111" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
-        <v>1454</v>
+      <c r="A111" s="4">
+        <v>45901</v>
       </c>
       <c r="B111" s="19" t="s">
         <v>1498</v>
@@ -34318,8 +34321,8 @@
       <c r="CO111" s="19"/>
     </row>
     <row r="112" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
-        <v>1454</v>
+      <c r="A112" s="4">
+        <v>45901</v>
       </c>
       <c r="B112" s="19" t="s">
         <v>1498</v>
@@ -34555,8 +34558,8 @@
       <c r="CO112" s="19"/>
     </row>
     <row r="113" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
-        <v>1454</v>
+      <c r="A113" s="4">
+        <v>45901</v>
       </c>
       <c r="B113" s="19" t="s">
         <v>1498</v>
@@ -34792,8 +34795,8 @@
       <c r="CO113" s="19"/>
     </row>
     <row r="114" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
-        <v>1454</v>
+      <c r="A114" s="4">
+        <v>45901</v>
       </c>
       <c r="B114" s="19" t="s">
         <v>502</v>
@@ -35027,8 +35030,8 @@
       <c r="CO114" s="19"/>
     </row>
     <row r="115" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
-        <v>1454</v>
+      <c r="A115" s="4">
+        <v>45901</v>
       </c>
       <c r="B115" s="19" t="s">
         <v>502</v>
@@ -35262,8 +35265,8 @@
       <c r="CO115" s="19"/>
     </row>
     <row r="116" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A116" s="4" t="s">
-        <v>1454</v>
+      <c r="A116" s="4">
+        <v>45901</v>
       </c>
       <c r="B116" s="19" t="s">
         <v>502</v>
@@ -35497,8 +35500,8 @@
       <c r="CO116" s="19"/>
     </row>
     <row r="117" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
-        <v>1454</v>
+      <c r="A117" s="4">
+        <v>45901</v>
       </c>
       <c r="B117" s="19" t="s">
         <v>502</v>

</xml_diff>